<commit_message>
02 - Especificação  do projeto
</commit_message>
<xml_diff>
--- a/Arquivos Design/Mapeamento HIstorias e Requisitos.xlsx
+++ b/Arquivos Design/Mapeamento HIstorias e Requisitos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suporte\Documents\GitHub\pmv-ads-2022-2-e2-proj-int-t7-pontoall\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suporte\Documents\GitHub\pmv-ads-2022-2-e2-proj-int-t7-pontoall\Arquivos Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8DFE14-5877-4C6B-9DAB-06EB01A17C96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0309C3F-87C8-459B-930E-C40041E384AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7906A824-BE43-47E1-94EC-881B8EB5B83E}"/>
   </bookViews>
@@ -755,40 +755,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1111,8 +1111,8 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,13 +1159,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="41" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="20" t="s">
@@ -1268,13 +1268,13 @@
       <c r="I6" s="29"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="36" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="21" t="s">
@@ -1394,13 +1394,13 @@
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="36" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="21" t="s">
@@ -1497,13 +1497,13 @@
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="36" t="s">
         <v>31</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -1642,18 +1642,18 @@
     <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="C18:C23"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="A18:A23"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
   </mergeCells>
   <pageMargins left="0.22" right="0.18" top="0.36" bottom="0.41" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="48" orientation="landscape" r:id="rId1"/>

</xml_diff>